<commit_message>
Finished visualization + changed "-" to "_" .xlsx
</commit_message>
<xml_diff>
--- a/Data/Techmap/DEModel.xlsx
+++ b/Data/Techmap/DEModel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sina Hajikazemi\Documents\mycode\demodel_pyomo\Data\Techmap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janwi\Desktop\5.Semester\Miniforschungsprojekt\Model_Deutschland_Sina\CESM\Data\Techmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D384D69-674A-4BD1-BC83-C1D4CF7CFB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A60DA33-3A9C-48CC-B80B-8056D30B6A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="120" windowWidth="6490" windowHeight="8170" activeTab="5" xr2:uid="{EC78BDD3-7137-425A-8228-7CE92A9A1C25}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{EC78BDD3-7137-425A-8228-7CE92A9A1C25}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="9" r:id="rId1"/>
@@ -731,9 +731,6 @@
     <t>Mio EUR</t>
   </si>
   <si>
-    <t>test-tss</t>
-  </si>
-  <si>
     <t>is_storage</t>
   </si>
   <si>
@@ -855,6 +852,9 @@
   </si>
   <si>
     <t>commodity_name</t>
+  </si>
+  <si>
+    <t>test_tss</t>
   </si>
 </sst>
 </file>
@@ -958,41 +958,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1396,23 +1384,23 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1423,7 +1411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1436,9 +1424,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B4" t="str">
         <f>IF(B2="kW","t",IF(B2="MW","kilo t","Mio t"))</f>
@@ -1448,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1460,7 +1448,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1472,7 +1460,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1484,9 +1472,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B8" t="s">
         <v>198</v>
@@ -1511,26 +1499,26 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" t="s">
         <v>224</v>
-      </c>
-      <c r="B1" t="s">
-        <v>225</v>
       </c>
       <c r="C1" t="s">
         <v>43</v>
@@ -1539,19 +1527,19 @@
         <v>44</v>
       </c>
       <c r="E1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" t="s">
         <v>226</v>
-      </c>
-      <c r="F1" t="s">
-        <v>239</v>
-      </c>
-      <c r="G1" t="s">
-        <v>227</v>
       </c>
       <c r="H1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1571,10 +1559,10 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>186</v>
       </c>
@@ -1591,10 +1579,10 @@
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>197</v>
       </c>
@@ -1617,7 +1605,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1637,7 +1625,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>181</v>
       </c>
@@ -1674,136 +1662,136 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>121</v>
       </c>
@@ -1821,280 +1809,280 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70369A52-6DA6-442B-A9B0-7FE85C1EDFA1}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>144</v>
       </c>
@@ -2113,60 +2101,60 @@
   <dimension ref="A1:Z88"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" customWidth="1"/>
-    <col min="4" max="5" width="10.81640625" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" customWidth="1"/>
-    <col min="7" max="9" width="10.81640625" customWidth="1"/>
-    <col min="10" max="10" width="20.26953125" customWidth="1"/>
-    <col min="11" max="12" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.81640625" customWidth="1"/>
-    <col min="14" max="14" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7265625" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="11" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="17.7265625" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" customWidth="1"/>
     <col min="18" max="18" width="30" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.7265625" customWidth="1"/>
-    <col min="20" max="20" width="13.1796875" customWidth="1"/>
-    <col min="21" max="21" width="14.1796875" customWidth="1"/>
-    <col min="22" max="22" width="14.453125" customWidth="1"/>
-    <col min="23" max="23" width="12.7265625" customWidth="1"/>
-    <col min="24" max="24" width="13.7265625" customWidth="1"/>
-    <col min="25" max="25" width="17.26953125" customWidth="1"/>
-    <col min="26" max="26" width="16.26953125" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="13.140625" customWidth="1"/>
+    <col min="21" max="21" width="14.140625" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" customWidth="1"/>
+    <col min="24" max="24" width="13.7109375" customWidth="1"/>
+    <col min="25" max="25" width="17.28515625" customWidth="1"/>
+    <col min="26" max="26" width="16.28515625" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" t="s">
         <v>232</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>233</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>234</v>
       </c>
-      <c r="D1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" t="s">
         <v>200</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>201</v>
       </c>
       <c r="H1" t="s">
         <v>40</v>
@@ -2220,75 +2208,72 @@
         <v>185</v>
       </c>
       <c r="Y1" t="s">
+        <v>207</v>
+      </c>
+      <c r="Z1" t="s">
         <v>208</v>
       </c>
-      <c r="Z1" t="s">
+    </row>
+    <row r="2" spans="1:26" s="5" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y2" s="5" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" s="7" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E2" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="X2" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y2" s="7" t="s">
+      <c r="Z2" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="Z2" s="7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+    </row>
+    <row r="3" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H3" s="1" t="s">
         <v>41</v>
       </c>
@@ -2329,32 +2314,32 @@
         <v>TWh/a</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="10"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="5"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="6"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="4"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>116</v>
       </c>
@@ -2370,33 +2355,33 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>0</v>
       </c>
       <c r="I5" s="3">
         <v>1</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="5"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="6">
+      <c r="J5" s="3"/>
+      <c r="K5" s="4"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="3">
         <v>20</v>
       </c>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="5">
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="4">
         <v>310</v>
       </c>
-      <c r="T5" s="6"/>
+      <c r="T5" s="3"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -2412,31 +2397,31 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>0.36</v>
       </c>
       <c r="I6" s="3">
         <v>1</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="5"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="6" t="s">
+      <c r="J6" s="3"/>
+      <c r="K6" s="4"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="6"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>117</v>
       </c>
@@ -2452,31 +2437,31 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>0.26</v>
       </c>
       <c r="I7" s="3">
         <v>1</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="5"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="6" t="s">
+      <c r="J7" s="3"/>
+      <c r="K7" s="4"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="6"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="3"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>119</v>
       </c>
@@ -2492,31 +2477,31 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>0.40400000000000003</v>
       </c>
       <c r="I8" s="3">
         <v>1</v>
       </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6" t="s">
+      <c r="J8" s="3"/>
+      <c r="K8" s="4"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="6"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>120</v>
       </c>
@@ -2532,31 +2517,31 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>0.2</v>
       </c>
       <c r="I9" s="3">
         <v>1</v>
       </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="5"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="6" t="s">
+      <c r="J9" s="3"/>
+      <c r="K9" s="4"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="6"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="3"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>122</v>
       </c>
@@ -2572,28 +2557,28 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>0</v>
       </c>
       <c r="I10" s="3">
         <v>1</v>
       </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="5"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="5"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="6"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="4"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="4"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="3"/>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>123</v>
       </c>
@@ -2609,30 +2594,30 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>0.28999999999999998</v>
       </c>
       <c r="I11" s="3">
         <v>1</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="5"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="5"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="5">
+      <c r="J11" s="3"/>
+      <c r="K11" s="4"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="4"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="4">
         <v>69</v>
       </c>
-      <c r="T11" s="6"/>
+      <c r="T11" s="3"/>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2641,22 +2626,22 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="5"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="5"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="6"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="4"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="4"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="3"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>124</v>
       </c>
@@ -2675,22 +2660,22 @@
       <c r="I13" s="3">
         <v>0.88</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="5"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="5"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="6"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="4"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="4"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="3"/>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="6"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2699,22 +2684,22 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="5"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="5"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="6"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="4"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="4"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>126</v>
       </c>
@@ -2733,25 +2718,25 @@
       <c r="I15" s="3">
         <v>1</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="5"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="5"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="T15" s="5">
+      <c r="J15" s="3"/>
+      <c r="K15" s="4"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="4"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="T15" s="4">
         <v>720</v>
       </c>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
-      <c r="Y15" s="6" t="s">
+      <c r="Y15" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Z15" s="6"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z15" s="3"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
@@ -2770,25 +2755,25 @@
       <c r="I16" s="3">
         <v>1</v>
       </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="5"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="5"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="T16" s="5">
+      <c r="J16" s="3"/>
+      <c r="K16" s="4"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="4"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="T16" s="4">
         <v>556</v>
       </c>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
-      <c r="Y16" s="6" t="s">
+      <c r="Y16" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="Z16" s="6"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z16" s="3"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>128</v>
       </c>
@@ -2807,25 +2792,25 @@
       <c r="I17" s="3">
         <v>1</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="5"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="5"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="T17" s="5">
+      <c r="J17" s="3"/>
+      <c r="K17" s="4"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="4"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="T17" s="4">
         <v>250</v>
       </c>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
-      <c r="Y17" s="6" t="s">
+      <c r="Y17" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Z17" s="6"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z17" s="3"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>130</v>
       </c>
@@ -2844,25 +2829,25 @@
       <c r="I18" s="3">
         <v>1</v>
       </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="5"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="5"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="T18" s="5">
+      <c r="J18" s="3"/>
+      <c r="K18" s="4"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="4"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="T18" s="4">
         <v>245</v>
       </c>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
-      <c r="Y18" s="6" t="s">
+      <c r="Y18" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Z18" s="6"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z18" s="3"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>132</v>
       </c>
@@ -2881,25 +2866,25 @@
       <c r="I19" s="3">
         <v>1</v>
       </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="5"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="5"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="T19" s="5">
+      <c r="J19" s="3"/>
+      <c r="K19" s="4"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="4"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="T19" s="4">
         <v>209</v>
       </c>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
-      <c r="Y19" s="6" t="s">
+      <c r="Y19" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Z19" s="6"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z19" s="3"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>134</v>
       </c>
@@ -2918,25 +2903,25 @@
       <c r="I20" s="3">
         <v>1</v>
       </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="5"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="5"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="T20" s="5">
+      <c r="J20" s="3"/>
+      <c r="K20" s="4"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="4"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="T20" s="4">
         <v>11</v>
       </c>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
-      <c r="Y20" s="6" t="s">
+      <c r="Y20" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Z20" s="6"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z20" s="3"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>135</v>
       </c>
@@ -2955,25 +2940,25 @@
       <c r="I21" s="3">
         <v>1</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="5"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="5"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="T21" s="5">
+      <c r="J21" s="3"/>
+      <c r="K21" s="4"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="4"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="T21" s="4">
         <v>135</v>
       </c>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
-      <c r="Y21" s="6" t="s">
+      <c r="Y21" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Z21" s="6"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z21" s="3"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2982,24 +2967,24 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="5"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="5"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="6"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="4"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="4"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="3"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="6"/>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>45</v>
@@ -3016,39 +3001,39 @@
       <c r="I23" s="3">
         <v>0.3</v>
       </c>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6" t="s">
+      <c r="J23" s="3"/>
+      <c r="K23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="L23" s="6" t="s">
+      <c r="L23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N23" s="6" t="s">
+      <c r="N23" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="O23" s="5">
+      <c r="O23" s="4">
         <v>30</v>
       </c>
-      <c r="Q23" s="6">
+      <c r="Q23" s="3">
         <v>165</v>
       </c>
-      <c r="R23" s="6">
+      <c r="R23" s="3">
         <v>3300</v>
       </c>
-      <c r="S23" s="5"/>
-      <c r="T23" s="6"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
-      <c r="Y23" s="6" t="s">
+      <c r="Y23" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Z23" s="6"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z23" s="3"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>18</v>
@@ -3065,39 +3050,39 @@
       <c r="I24" s="3">
         <v>0.38</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J24" s="3">
         <v>0.75</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="K24" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="L24" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="N24" s="6" t="s">
+      <c r="N24" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="O24" s="5">
+      <c r="O24" s="4">
         <v>40</v>
       </c>
-      <c r="Q24" s="6">
+      <c r="Q24" s="3">
         <v>20</v>
       </c>
-      <c r="R24" s="6">
+      <c r="R24" s="3">
         <v>1500</v>
       </c>
-      <c r="S24" s="5"/>
-      <c r="T24" s="6"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="6"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>121</v>
@@ -3114,39 +3099,39 @@
       <c r="I25" s="3">
         <v>0.4</v>
       </c>
-      <c r="J25" s="6">
+      <c r="J25" s="3">
         <v>0.95</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="K25" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="L25" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="N25" s="6" t="s">
+      <c r="N25" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="O25" s="5">
+      <c r="O25" s="4">
         <v>25</v>
       </c>
-      <c r="Q25" s="6">
+      <c r="Q25" s="3">
         <v>14.25</v>
       </c>
-      <c r="R25" s="6">
+      <c r="R25" s="3">
         <v>400</v>
       </c>
-      <c r="S25" s="5"/>
-      <c r="T25" s="6"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
-      <c r="Y25" s="6"/>
-      <c r="Z25" s="6"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>48</v>
@@ -3163,39 +3148,39 @@
       <c r="I26" s="3">
         <v>0.35</v>
       </c>
-      <c r="J26" s="6">
+      <c r="J26" s="3">
         <v>0.75</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="K26" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="L26" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="N26" s="6" t="s">
+      <c r="N26" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="O26" s="5">
+      <c r="O26" s="4">
         <v>40</v>
       </c>
-      <c r="Q26" s="6">
+      <c r="Q26" s="3">
         <v>50</v>
       </c>
-      <c r="R26" s="6">
+      <c r="R26" s="3">
         <v>1600</v>
       </c>
-      <c r="S26" s="5"/>
-      <c r="T26" s="6"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
-      <c r="Y26" s="6"/>
-      <c r="Z26" s="6"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>47</v>
@@ -3212,37 +3197,37 @@
       <c r="I27" s="3">
         <v>0.33</v>
       </c>
-      <c r="J27" s="6">
+      <c r="J27" s="3">
         <v>0.98</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="K27" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="L27" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="N27" s="6" t="s">
+      <c r="N27" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="O27" s="5">
+      <c r="O27" s="4">
         <v>60</v>
       </c>
-      <c r="Q27" s="6">
+      <c r="Q27" s="3">
         <v>102</v>
       </c>
-      <c r="R27" s="6">
+      <c r="R27" s="3">
         <v>3323</v>
       </c>
-      <c r="S27" s="5"/>
-      <c r="T27" s="6"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="3"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
-      <c r="Y27" s="6"/>
-      <c r="Z27" s="6"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -3251,25 +3236,25 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="5"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="6"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="4"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="3"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
-      <c r="Y28" s="6"/>
-      <c r="Z28" s="6"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>17</v>
@@ -3286,37 +3271,37 @@
       <c r="I29" s="3">
         <v>1</v>
       </c>
-      <c r="J29" s="6"/>
-      <c r="K29" s="5" t="s">
+      <c r="J29" s="3"/>
+      <c r="K29" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="L29" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="N29" s="5" t="s">
+      <c r="N29" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="O29" s="5">
+      <c r="O29" s="4">
         <v>25</v>
       </c>
-      <c r="Q29" s="6" t="s">
+      <c r="Q29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="R29" s="6" t="s">
+      <c r="R29" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="S29" s="5"/>
-      <c r="T29" s="6"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="3"/>
       <c r="U29" s="3"/>
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
-      <c r="Y29" s="6"/>
-      <c r="Z29" s="6" t="s">
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>136</v>
       </c>
@@ -3335,35 +3320,35 @@
       <c r="I30" s="3">
         <v>1</v>
       </c>
-      <c r="J30" s="6"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="N30" s="6" t="s">
+      <c r="J30" s="3"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="N30" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="O30" s="5">
+      <c r="O30" s="4">
         <v>25</v>
       </c>
-      <c r="Q30" s="6">
+      <c r="Q30" s="3">
         <v>93</v>
       </c>
-      <c r="R30" s="6" t="s">
+      <c r="R30" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="S30" s="5"/>
-      <c r="T30" s="6"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="3"/>
       <c r="U30" s="3"/>
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
-      <c r="Y30" s="6"/>
-      <c r="Z30" s="6" t="s">
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>17</v>
@@ -3380,37 +3365,37 @@
       <c r="I31" s="3">
         <v>1</v>
       </c>
-      <c r="J31" s="6"/>
-      <c r="K31" s="5" t="s">
+      <c r="J31" s="3"/>
+      <c r="K31" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="L31" s="5" t="s">
+      <c r="L31" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="N31" s="5" t="s">
+      <c r="N31" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="O31" s="5">
+      <c r="O31" s="4">
         <v>25</v>
       </c>
-      <c r="Q31" s="6" t="s">
+      <c r="Q31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="R31" s="6" t="s">
+      <c r="R31" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S31" s="5"/>
-      <c r="T31" s="6"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="3"/>
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
-      <c r="Y31" s="6"/>
-      <c r="Z31" s="6" t="s">
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>137</v>
       </c>
@@ -3429,37 +3414,37 @@
       <c r="I32" s="3">
         <v>1</v>
       </c>
-      <c r="J32" s="6"/>
-      <c r="K32" s="5">
-        <v>0</v>
-      </c>
-      <c r="L32" s="5">
-        <v>0</v>
-      </c>
-      <c r="N32" s="6" t="s">
+      <c r="J32" s="3"/>
+      <c r="K32" s="4">
+        <v>0</v>
+      </c>
+      <c r="L32" s="4">
+        <v>0</v>
+      </c>
+      <c r="N32" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="O32" s="5">
+      <c r="O32" s="4">
         <v>25</v>
       </c>
-      <c r="Q32" s="6">
+      <c r="Q32" s="3">
         <v>13</v>
       </c>
-      <c r="R32" s="6" t="s">
+      <c r="R32" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="S32" s="5"/>
-      <c r="T32" s="6"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="3"/>
       <c r="U32" s="3"/>
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
-      <c r="Y32" s="6"/>
-      <c r="Z32" s="6" t="s">
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>138</v>
       </c>
@@ -3478,41 +3463,41 @@
       <c r="I33" s="3">
         <v>1</v>
       </c>
-      <c r="J33" s="6"/>
-      <c r="K33" s="5">
+      <c r="J33" s="3"/>
+      <c r="K33" s="4">
         <v>3.8388200000000001</v>
       </c>
-      <c r="L33" s="5">
+      <c r="L33" s="4">
         <v>3.8388200000000001</v>
       </c>
-      <c r="N33" s="5">
+      <c r="N33" s="4">
         <v>3.8388200000000001</v>
       </c>
-      <c r="O33" s="5">
+      <c r="O33" s="4">
         <v>100</v>
       </c>
-      <c r="Q33" s="6">
+      <c r="Q33" s="3">
         <v>12</v>
       </c>
-      <c r="R33" s="6">
+      <c r="R33" s="3">
         <v>5000</v>
       </c>
-      <c r="S33" s="5" t="s">
+      <c r="S33" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="T33" s="6"/>
+      <c r="T33" s="3"/>
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
-      <c r="Y33" s="6" t="s">
+      <c r="Y33" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Z33" s="6"/>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z33" s="3"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>17</v>
@@ -3529,37 +3514,37 @@
       <c r="I34" s="3">
         <v>1</v>
       </c>
-      <c r="J34" s="6"/>
-      <c r="K34" s="5" t="s">
+      <c r="J34" s="3"/>
+      <c r="K34" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="L34" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="N34" s="5" t="s">
+      <c r="N34" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O34" s="5">
+      <c r="O34" s="4">
         <v>30</v>
       </c>
-      <c r="Q34" s="6">
+      <c r="Q34" s="3">
         <v>30</v>
       </c>
-      <c r="R34" s="6" t="s">
+      <c r="R34" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="S34" s="5"/>
-      <c r="T34" s="6"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="3"/>
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
-      <c r="Y34" s="6"/>
-      <c r="Z34" s="6" t="s">
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>139</v>
       </c>
@@ -3578,37 +3563,37 @@
       <c r="I35" s="3">
         <v>1</v>
       </c>
-      <c r="J35" s="6"/>
-      <c r="K35" s="5">
-        <v>0</v>
-      </c>
-      <c r="L35" s="5">
-        <v>0</v>
-      </c>
-      <c r="N35" s="6" t="s">
+      <c r="J35" s="3"/>
+      <c r="K35" s="4">
+        <v>0</v>
+      </c>
+      <c r="L35" s="4">
+        <v>0</v>
+      </c>
+      <c r="N35" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="O35" s="5">
+      <c r="O35" s="4">
         <v>25</v>
       </c>
-      <c r="Q35" s="6">
+      <c r="Q35" s="3">
         <v>15</v>
       </c>
-      <c r="R35" s="6" t="s">
+      <c r="R35" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="S35" s="5"/>
-      <c r="T35" s="6"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="3"/>
       <c r="U35" s="3"/>
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
-      <c r="Y35" s="6"/>
-      <c r="Z35" s="9" t="s">
+      <c r="Y35" s="3"/>
+      <c r="Z35" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -3617,22 +3602,22 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="I36" s="3"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="5"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="5"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="6"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="4"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="4"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="3"/>
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
-      <c r="Y36" s="6"/>
-      <c r="Z36" s="6"/>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>140</v>
       </c>
@@ -3651,32 +3636,32 @@
       <c r="I37" s="3">
         <v>0.85</v>
       </c>
-      <c r="J37" s="6"/>
-      <c r="K37" s="5"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="5">
+      <c r="J37" s="3"/>
+      <c r="K37" s="4"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="4">
         <v>15</v>
       </c>
-      <c r="Q37" s="6" t="s">
+      <c r="Q37" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="R37" s="6">
+      <c r="R37" s="3">
         <v>220</v>
       </c>
-      <c r="S37" s="5">
+      <c r="S37" s="4">
         <v>120</v>
       </c>
-      <c r="T37" s="5">
+      <c r="T37" s="4">
         <v>70</v>
       </c>
       <c r="U37" s="3"/>
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
-      <c r="Y37" s="6"/>
-      <c r="Z37" s="6"/>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y37" s="3"/>
+      <c r="Z37" s="3"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>141</v>
       </c>
@@ -3695,28 +3680,28 @@
       <c r="I38" s="3">
         <v>0.95</v>
       </c>
-      <c r="J38" s="6"/>
-      <c r="K38" s="5"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="5">
+      <c r="J38" s="3"/>
+      <c r="K38" s="4"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="4">
         <v>15</v>
       </c>
-      <c r="Q38" s="6" t="s">
+      <c r="Q38" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="R38" s="6">
+      <c r="R38" s="3">
         <v>15</v>
       </c>
-      <c r="S38" s="5"/>
-      <c r="T38" s="6"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="3"/>
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
-      <c r="Y38" s="6"/>
-      <c r="Z38" s="6"/>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>142</v>
       </c>
@@ -3735,32 +3720,32 @@
       <c r="I39" s="3">
         <v>1</v>
       </c>
-      <c r="J39" s="6"/>
-      <c r="K39" s="5"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="5">
+      <c r="J39" s="3"/>
+      <c r="K39" s="4"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="4">
         <v>12.5</v>
       </c>
-      <c r="Q39" s="6">
-        <v>0</v>
-      </c>
-      <c r="R39" s="6">
+      <c r="Q39" s="3">
+        <v>0</v>
+      </c>
+      <c r="R39" s="3">
         <v>60</v>
       </c>
-      <c r="S39" s="5"/>
-      <c r="T39" s="6">
+      <c r="S39" s="4"/>
+      <c r="T39" s="3">
         <v>40.061100000000003</v>
       </c>
       <c r="U39" s="3"/>
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
-      <c r="Y39" s="6" t="s">
+      <c r="Y39" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Z39" s="6"/>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z39" s="3"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -3769,22 +3754,22 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="5"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="5"/>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="6"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="4"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="4"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="3"/>
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
       <c r="X40" s="3"/>
-      <c r="Y40" s="6"/>
-      <c r="Z40" s="6"/>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y40" s="3"/>
+      <c r="Z40" s="3"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>143</v>
       </c>
@@ -3801,22 +3786,22 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="I41" s="3"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="5"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="5"/>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="6"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="4"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="4"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="3"/>
       <c r="U41" s="3"/>
       <c r="V41" s="3"/>
       <c r="W41" s="3"/>
       <c r="X41" s="3"/>
-      <c r="Y41" s="6"/>
-      <c r="Z41" s="6"/>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y41" s="3"/>
+      <c r="Z41" s="3"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -3825,22 +3810,22 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="I42" s="3"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="5"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="5"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="6"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="4"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="4"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="3"/>
       <c r="U42" s="3"/>
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
       <c r="X42" s="3"/>
-      <c r="Y42" s="6"/>
-      <c r="Z42" s="6"/>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>144</v>
       </c>
@@ -3859,30 +3844,30 @@
       <c r="I43" s="3">
         <v>0.7</v>
       </c>
-      <c r="J43" s="6"/>
-      <c r="K43" s="5"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="5">
+      <c r="J43" s="3"/>
+      <c r="K43" s="4"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="4">
         <v>15</v>
       </c>
-      <c r="Q43" s="6" t="s">
+      <c r="Q43" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="R43" s="6">
+      <c r="R43" s="3">
         <v>220</v>
       </c>
-      <c r="S43" s="5"/>
-      <c r="T43" s="6"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="3"/>
       <c r="U43" s="3"/>
       <c r="V43" s="3"/>
       <c r="W43" s="3"/>
       <c r="X43" s="3"/>
-      <c r="Y43" s="6" t="s">
+      <c r="Y43" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Z43" s="6"/>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z43" s="3"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>145</v>
       </c>
@@ -3901,28 +3886,28 @@
       <c r="I44" s="3">
         <v>0.8</v>
       </c>
-      <c r="J44" s="6"/>
-      <c r="K44" s="5"/>
-      <c r="N44" s="6"/>
-      <c r="O44" s="5">
+      <c r="J44" s="3"/>
+      <c r="K44" s="4"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="4">
         <v>15</v>
       </c>
-      <c r="Q44" s="6" t="s">
+      <c r="Q44" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="R44" s="6">
+      <c r="R44" s="3">
         <v>220</v>
       </c>
-      <c r="S44" s="5"/>
-      <c r="T44" s="6"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="3"/>
       <c r="U44" s="3"/>
       <c r="V44" s="3"/>
       <c r="W44" s="3"/>
       <c r="X44" s="3"/>
-      <c r="Y44" s="6"/>
-      <c r="Z44" s="6"/>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y44" s="3"/>
+      <c r="Z44" s="3"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>146</v>
       </c>
@@ -3941,28 +3926,28 @@
       <c r="I45" s="3">
         <v>3.2</v>
       </c>
-      <c r="J45" s="6"/>
-      <c r="K45" s="5"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="5">
+      <c r="J45" s="3"/>
+      <c r="K45" s="4"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="4">
         <v>25</v>
       </c>
-      <c r="Q45" s="6">
+      <c r="Q45" s="3">
         <v>2</v>
       </c>
-      <c r="R45" s="6" t="s">
+      <c r="R45" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="S45" s="5"/>
-      <c r="T45" s="6"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="3"/>
       <c r="U45" s="3"/>
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
       <c r="X45" s="3"/>
-      <c r="Y45" s="6"/>
-      <c r="Z45" s="6"/>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y45" s="3"/>
+      <c r="Z45" s="3"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -3971,22 +3956,22 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="I46" s="3"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="5"/>
-      <c r="N46" s="6"/>
-      <c r="O46" s="5"/>
-      <c r="Q46" s="6"/>
-      <c r="R46" s="6"/>
-      <c r="S46" s="5"/>
-      <c r="T46" s="6"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="4"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="4"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="3"/>
       <c r="U46" s="3"/>
       <c r="V46" s="3"/>
       <c r="W46" s="3"/>
       <c r="X46" s="3"/>
-      <c r="Y46" s="6"/>
-      <c r="Z46" s="6"/>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y46" s="3"/>
+      <c r="Z46" s="3"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -3995,22 +3980,22 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="I47" s="3"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="5"/>
-      <c r="N47" s="6"/>
-      <c r="O47" s="5"/>
-      <c r="Q47" s="6"/>
-      <c r="R47" s="6"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="6"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="4"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="4"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="3"/>
       <c r="U47" s="3"/>
       <c r="V47" s="3"/>
       <c r="W47" s="3"/>
       <c r="X47" s="3"/>
-      <c r="Y47" s="6"/>
-      <c r="Z47" s="6"/>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y47" s="3"/>
+      <c r="Z47" s="3"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>147</v>
       </c>
@@ -4029,35 +4014,35 @@
       <c r="I48" s="3">
         <v>0.9</v>
       </c>
-      <c r="J48" s="6"/>
-      <c r="K48" s="5" t="s">
+      <c r="J48" s="3"/>
+      <c r="K48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L48" s="5" t="s">
+      <c r="L48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="N48" s="5" t="s">
+      <c r="N48" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="O48" s="5">
+      <c r="O48" s="4">
         <v>25</v>
       </c>
-      <c r="Q48" s="6" t="s">
+      <c r="Q48" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="R48" s="6" t="s">
+      <c r="R48" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="S48" s="5"/>
-      <c r="T48" s="6"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="3"/>
       <c r="U48" s="3"/>
       <c r="V48" s="3"/>
       <c r="W48" s="3"/>
       <c r="X48" s="3"/>
-      <c r="Y48" s="6"/>
-      <c r="Z48" s="6"/>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y48" s="3"/>
+      <c r="Z48" s="3"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -4066,23 +4051,23 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="I49" s="3"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="5"/>
-      <c r="Q49" s="6"/>
-      <c r="R49" s="6"/>
-      <c r="S49" s="5"/>
-      <c r="T49" s="6"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="3"/>
       <c r="U49" s="3"/>
       <c r="V49" s="3"/>
       <c r="W49" s="3"/>
       <c r="X49" s="3"/>
-      <c r="Y49" s="6"/>
-      <c r="Z49" s="6"/>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y49" s="3"/>
+      <c r="Z49" s="3"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>149</v>
       </c>
@@ -4101,35 +4086,35 @@
       <c r="I50" s="3">
         <v>0.85</v>
       </c>
-      <c r="J50" s="6"/>
-      <c r="K50" s="5" t="s">
+      <c r="J50" s="3"/>
+      <c r="K50" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L50" s="5" t="s">
+      <c r="L50" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="N50" s="5" t="s">
+      <c r="N50" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="O50" s="5">
+      <c r="O50" s="4">
         <v>20</v>
       </c>
-      <c r="Q50" s="6">
+      <c r="Q50" s="3">
         <v>44</v>
       </c>
-      <c r="R50" s="6" t="s">
+      <c r="R50" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="S50" s="5"/>
-      <c r="T50" s="6"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="3"/>
       <c r="U50" s="3"/>
       <c r="V50" s="3"/>
       <c r="W50" s="3"/>
       <c r="X50" s="3"/>
-      <c r="Y50" s="6"/>
-      <c r="Z50" s="6"/>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y50" s="3"/>
+      <c r="Z50" s="3"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>151</v>
       </c>
@@ -4148,35 +4133,35 @@
       <c r="I51" s="3">
         <v>0.9</v>
       </c>
-      <c r="J51" s="6"/>
-      <c r="K51" s="5" t="s">
+      <c r="J51" s="3"/>
+      <c r="K51" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="L51" s="5" t="s">
+      <c r="L51" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="N51" s="5" t="s">
+      <c r="N51" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="O51" s="5">
+      <c r="O51" s="4">
         <v>20</v>
       </c>
-      <c r="Q51" s="6" t="s">
+      <c r="Q51" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="R51" s="6" t="s">
+      <c r="R51" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="S51" s="5"/>
-      <c r="T51" s="6"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="3"/>
       <c r="U51" s="3"/>
       <c r="V51" s="3"/>
       <c r="W51" s="3"/>
       <c r="X51" s="3"/>
-      <c r="Y51" s="6"/>
-      <c r="Z51" s="6"/>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y51" s="3"/>
+      <c r="Z51" s="3"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>153</v>
       </c>
@@ -4195,35 +4180,35 @@
       <c r="I52" s="3">
         <v>3.5</v>
       </c>
-      <c r="J52" s="6"/>
-      <c r="K52" s="5">
-        <v>0</v>
-      </c>
-      <c r="L52" s="5">
-        <v>0</v>
-      </c>
-      <c r="N52" s="5" t="s">
+      <c r="J52" s="3"/>
+      <c r="K52" s="4">
+        <v>0</v>
+      </c>
+      <c r="L52" s="4">
+        <v>0</v>
+      </c>
+      <c r="N52" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="O52" s="5">
+      <c r="O52" s="4">
         <v>20</v>
       </c>
-      <c r="Q52" s="6" t="s">
+      <c r="Q52" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="R52" s="6" t="s">
+      <c r="R52" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="S52" s="5"/>
-      <c r="T52" s="6"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="3"/>
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
       <c r="X52" s="3"/>
-      <c r="Y52" s="6"/>
-      <c r="Z52" s="6"/>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y52" s="3"/>
+      <c r="Z52" s="3"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>155</v>
       </c>
@@ -4242,35 +4227,35 @@
       <c r="I53" s="3">
         <v>0.85</v>
       </c>
-      <c r="J53" s="6"/>
-      <c r="K53" s="5" t="s">
+      <c r="J53" s="3"/>
+      <c r="K53" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="L53" s="5" t="s">
+      <c r="L53" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="N53" s="5" t="s">
+      <c r="N53" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="O53" s="5">
+      <c r="O53" s="4">
         <v>20</v>
       </c>
-      <c r="Q53" s="6" t="s">
+      <c r="Q53" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="R53" s="6" t="s">
+      <c r="R53" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="S53" s="5"/>
-      <c r="T53" s="6"/>
+      <c r="S53" s="4"/>
+      <c r="T53" s="3"/>
       <c r="U53" s="3"/>
       <c r="V53" s="3"/>
       <c r="W53" s="3"/>
       <c r="X53" s="3"/>
-      <c r="Y53" s="6"/>
-      <c r="Z53" s="6"/>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y53" s="3"/>
+      <c r="Z53" s="3"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>157</v>
       </c>
@@ -4289,30 +4274,30 @@
       <c r="I54" s="3">
         <v>1</v>
       </c>
-      <c r="J54" s="6"/>
-      <c r="K54" s="5"/>
-      <c r="N54" s="6" t="s">
+      <c r="J54" s="3"/>
+      <c r="K54" s="4"/>
+      <c r="N54" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="O54" s="5">
+      <c r="O54" s="4">
         <v>30</v>
       </c>
-      <c r="Q54" s="6" t="s">
+      <c r="Q54" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="R54" s="6" t="s">
+      <c r="R54" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="S54" s="5"/>
-      <c r="T54" s="6"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="3"/>
       <c r="U54" s="3"/>
       <c r="V54" s="3"/>
       <c r="W54" s="3"/>
       <c r="X54" s="3"/>
-      <c r="Y54" s="6"/>
-      <c r="Z54" s="6"/>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y54" s="3"/>
+      <c r="Z54" s="3"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>157</v>
       </c>
@@ -4331,30 +4316,30 @@
       <c r="I55" s="3">
         <v>1</v>
       </c>
-      <c r="J55" s="6"/>
-      <c r="K55" s="5"/>
-      <c r="N55" s="6" t="s">
+      <c r="J55" s="3"/>
+      <c r="K55" s="4"/>
+      <c r="N55" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="O55" s="5">
+      <c r="O55" s="4">
         <v>30</v>
       </c>
-      <c r="Q55" s="6" t="s">
+      <c r="Q55" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="R55" s="6" t="s">
+      <c r="R55" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="S55" s="5"/>
-      <c r="T55" s="6"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="3"/>
       <c r="U55" s="3"/>
       <c r="V55" s="3"/>
       <c r="W55" s="3"/>
       <c r="X55" s="3"/>
-      <c r="Y55" s="6"/>
-      <c r="Z55" s="6"/>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y55" s="3"/>
+      <c r="Z55" s="3"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>157</v>
       </c>
@@ -4373,30 +4358,30 @@
       <c r="I56" s="3">
         <v>1</v>
       </c>
-      <c r="J56" s="6"/>
-      <c r="K56" s="5"/>
-      <c r="N56" s="6" t="s">
+      <c r="J56" s="3"/>
+      <c r="K56" s="4"/>
+      <c r="N56" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="O56" s="5">
+      <c r="O56" s="4">
         <v>30</v>
       </c>
-      <c r="Q56" s="6" t="s">
+      <c r="Q56" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="R56" s="6" t="s">
+      <c r="R56" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="S56" s="5"/>
-      <c r="T56" s="6"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="3"/>
       <c r="U56" s="3"/>
       <c r="V56" s="3"/>
       <c r="W56" s="3"/>
       <c r="X56" s="3"/>
-      <c r="Y56" s="6"/>
-      <c r="Z56" s="6"/>
-    </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y56" s="3"/>
+      <c r="Z56" s="3"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>157</v>
       </c>
@@ -4415,30 +4400,30 @@
       <c r="I57" s="3">
         <v>1</v>
       </c>
-      <c r="J57" s="6"/>
-      <c r="K57" s="5"/>
-      <c r="N57" s="6" t="s">
+      <c r="J57" s="3"/>
+      <c r="K57" s="4"/>
+      <c r="N57" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="O57" s="5">
+      <c r="O57" s="4">
         <v>30</v>
       </c>
-      <c r="Q57" s="6" t="s">
+      <c r="Q57" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="R57" s="6" t="s">
+      <c r="R57" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="S57" s="5"/>
-      <c r="T57" s="6"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="3"/>
       <c r="U57" s="3"/>
       <c r="V57" s="3"/>
       <c r="W57" s="3"/>
       <c r="X57" s="3"/>
-      <c r="Y57" s="6"/>
-      <c r="Z57" s="6"/>
-    </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y57" s="3"/>
+      <c r="Z57" s="3"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>157</v>
       </c>
@@ -4457,28 +4442,28 @@
       <c r="I58" s="3">
         <v>1</v>
       </c>
-      <c r="J58" s="6"/>
-      <c r="K58" s="5"/>
-      <c r="N58" s="6"/>
-      <c r="O58" s="5">
+      <c r="J58" s="3"/>
+      <c r="K58" s="4"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="4">
         <v>30</v>
       </c>
-      <c r="Q58" s="6" t="s">
+      <c r="Q58" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="R58" s="6" t="s">
+      <c r="R58" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="S58" s="5"/>
-      <c r="T58" s="6"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="3"/>
       <c r="U58" s="3"/>
       <c r="V58" s="3"/>
       <c r="W58" s="3"/>
       <c r="X58" s="3"/>
-      <c r="Y58" s="6"/>
-      <c r="Z58" s="6"/>
-    </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y58" s="3"/>
+      <c r="Z58" s="3"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -4487,22 +4472,22 @@
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="I59" s="3"/>
-      <c r="J59" s="6"/>
-      <c r="K59" s="5"/>
-      <c r="N59" s="6"/>
-      <c r="O59" s="5"/>
-      <c r="Q59" s="6"/>
-      <c r="R59" s="6"/>
-      <c r="S59" s="5"/>
-      <c r="T59" s="6"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="4"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="4"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="4"/>
+      <c r="T59" s="3"/>
       <c r="U59" s="3"/>
       <c r="V59" s="3"/>
       <c r="W59" s="3"/>
       <c r="X59" s="3"/>
-      <c r="Y59" s="6"/>
-      <c r="Z59" s="6"/>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y59" s="3"/>
+      <c r="Z59" s="3"/>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>159</v>
       </c>
@@ -4519,26 +4504,26 @@
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="I60" s="3"/>
-      <c r="J60" s="6"/>
-      <c r="K60" s="5"/>
-      <c r="N60" s="6"/>
-      <c r="O60" s="5"/>
-      <c r="Q60" s="6"/>
-      <c r="R60" s="6"/>
-      <c r="S60" s="5"/>
-      <c r="T60" s="6"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="4"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="4"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="3"/>
       <c r="U60" s="3" t="s">
         <v>108</v>
       </c>
       <c r="V60" s="3"/>
       <c r="W60" s="3"/>
       <c r="X60" s="3"/>
-      <c r="Y60" s="6" t="s">
+      <c r="Y60" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Z60" s="6"/>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z60" s="3"/>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>160</v>
       </c>
@@ -4557,14 +4542,14 @@
       <c r="I61" s="3">
         <v>1</v>
       </c>
-      <c r="J61" s="6"/>
-      <c r="K61" s="5"/>
-      <c r="N61" s="6"/>
-      <c r="O61" s="5"/>
-      <c r="Q61" s="6"/>
-      <c r="R61" s="6"/>
-      <c r="S61" s="5"/>
-      <c r="T61" s="6"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="4"/>
+      <c r="N61" s="3"/>
+      <c r="O61" s="4"/>
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="4"/>
+      <c r="T61" s="3"/>
       <c r="U61" s="3" t="s">
         <v>108</v>
       </c>
@@ -4573,12 +4558,12 @@
       </c>
       <c r="W61" s="3"/>
       <c r="X61" s="3"/>
-      <c r="Y61" s="6" t="s">
+      <c r="Y61" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Z61" s="6"/>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z61" s="3"/>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>161</v>
       </c>
@@ -4595,26 +4580,26 @@
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="I62" s="3"/>
-      <c r="J62" s="6"/>
-      <c r="K62" s="5"/>
-      <c r="N62" s="6"/>
-      <c r="O62" s="5"/>
-      <c r="Q62" s="6"/>
-      <c r="R62" s="6"/>
-      <c r="S62" s="5"/>
-      <c r="T62" s="6"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="4"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="4"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="3"/>
       <c r="U62" s="3" t="s">
         <v>110</v>
       </c>
       <c r="V62" s="3"/>
       <c r="W62" s="3"/>
       <c r="X62" s="3"/>
-      <c r="Y62" s="6" t="s">
+      <c r="Y62" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Z62" s="6"/>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z62" s="3"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>162</v>
       </c>
@@ -4631,24 +4616,24 @@
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="I63" s="3"/>
-      <c r="J63" s="6"/>
-      <c r="K63" s="5"/>
-      <c r="N63" s="6"/>
-      <c r="O63" s="5"/>
-      <c r="Q63" s="6"/>
-      <c r="R63" s="6"/>
-      <c r="S63" s="5"/>
-      <c r="T63" s="6"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="4"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="4"/>
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="4"/>
+      <c r="T63" s="3"/>
       <c r="U63" s="3"/>
       <c r="V63" s="3"/>
       <c r="W63" s="3"/>
       <c r="X63" s="3"/>
-      <c r="Y63" s="6" t="s">
+      <c r="Y63" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Z63" s="6"/>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z63" s="3"/>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>163</v>
       </c>
@@ -4665,26 +4650,26 @@
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="I64" s="3"/>
-      <c r="J64" s="6"/>
-      <c r="K64" s="5"/>
-      <c r="N64" s="6"/>
-      <c r="O64" s="5"/>
-      <c r="Q64" s="6"/>
-      <c r="R64" s="6"/>
-      <c r="S64" s="5"/>
-      <c r="T64" s="6"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="4"/>
+      <c r="N64" s="3"/>
+      <c r="O64" s="4"/>
+      <c r="Q64" s="3"/>
+      <c r="R64" s="3"/>
+      <c r="S64" s="4"/>
+      <c r="T64" s="3"/>
       <c r="U64" s="3" t="s">
         <v>111</v>
       </c>
       <c r="V64" s="3"/>
       <c r="W64" s="3"/>
       <c r="X64" s="3"/>
-      <c r="Y64" s="6" t="s">
+      <c r="Y64" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Z64" s="6"/>
-    </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z64" s="3"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>164</v>
       </c>
@@ -4701,26 +4686,26 @@
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
       <c r="I65" s="3"/>
-      <c r="J65" s="6"/>
-      <c r="K65" s="5"/>
-      <c r="N65" s="6"/>
-      <c r="O65" s="5"/>
-      <c r="Q65" s="6"/>
-      <c r="R65" s="6"/>
-      <c r="S65" s="5"/>
-      <c r="T65" s="6"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="4"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="4"/>
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="4"/>
+      <c r="T65" s="3"/>
       <c r="U65" s="3" t="s">
         <v>112</v>
       </c>
       <c r="V65" s="3"/>
       <c r="W65" s="3"/>
       <c r="X65" s="3"/>
-      <c r="Y65" s="6" t="s">
+      <c r="Y65" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Z65" s="6"/>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z65" s="3"/>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -4729,24 +4714,24 @@
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
       <c r="I66" s="3"/>
-      <c r="J66" s="6"/>
-      <c r="K66" s="5"/>
-      <c r="N66" s="6"/>
-      <c r="O66" s="5"/>
-      <c r="Q66" s="6"/>
-      <c r="R66" s="6"/>
-      <c r="S66" s="5"/>
-      <c r="T66" s="6"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="4"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="4"/>
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="4"/>
+      <c r="T66" s="3"/>
       <c r="U66" s="3"/>
       <c r="V66" s="3"/>
       <c r="W66" s="3"/>
       <c r="X66" s="3"/>
-      <c r="Y66" s="6"/>
-      <c r="Z66" s="6"/>
-    </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y66" s="3"/>
+      <c r="Z66" s="3"/>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>45</v>
@@ -4763,32 +4748,32 @@
       <c r="I67" s="3">
         <v>1</v>
       </c>
-      <c r="J67" s="6">
+      <c r="J67" s="3">
         <v>0.99</v>
       </c>
-      <c r="K67" s="5"/>
-      <c r="N67" s="6"/>
-      <c r="O67" s="5">
+      <c r="K67" s="4"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="4">
         <v>30</v>
       </c>
-      <c r="Q67" s="6" t="s">
+      <c r="Q67" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="R67" s="6" t="s">
+      <c r="R67" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="S67" s="5"/>
-      <c r="T67" s="6"/>
+      <c r="S67" s="4"/>
+      <c r="T67" s="3"/>
       <c r="U67" s="3"/>
       <c r="V67" s="3"/>
       <c r="W67" s="3"/>
       <c r="X67" s="3"/>
-      <c r="Y67" s="6"/>
-      <c r="Z67" s="6"/>
-    </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y67" s="3"/>
+      <c r="Z67" s="3"/>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>165</v>
@@ -4803,26 +4788,26 @@
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
       <c r="I68" s="3"/>
-      <c r="J68" s="6"/>
-      <c r="K68" s="5"/>
-      <c r="N68" s="6"/>
-      <c r="O68" s="5"/>
-      <c r="Q68" s="6"/>
-      <c r="R68" s="6"/>
-      <c r="S68" s="5"/>
-      <c r="T68" s="6"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="4"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="4"/>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="4"/>
+      <c r="T68" s="3"/>
       <c r="U68" s="3"/>
       <c r="V68" s="3"/>
       <c r="W68" s="3">
         <v>0.2</v>
       </c>
       <c r="X68" s="3"/>
-      <c r="Y68" s="6"/>
-      <c r="Z68" s="6"/>
-    </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y68" s="3"/>
+      <c r="Z68" s="3"/>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>165</v>
@@ -4837,18 +4822,18 @@
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="I69" s="3"/>
-      <c r="J69" s="6"/>
-      <c r="K69" s="5">
+      <c r="J69" s="3"/>
+      <c r="K69" s="4">
         <v>3.5</v>
       </c>
-      <c r="N69" s="6">
+      <c r="N69" s="3">
         <v>3.5</v>
       </c>
-      <c r="O69" s="5"/>
-      <c r="Q69" s="6"/>
-      <c r="R69" s="6"/>
-      <c r="S69" s="5"/>
-      <c r="T69" s="6"/>
+      <c r="O69" s="4"/>
+      <c r="Q69" s="3"/>
+      <c r="R69" s="3"/>
+      <c r="S69" s="4"/>
+      <c r="T69" s="3"/>
       <c r="U69" s="3"/>
       <c r="V69" s="3"/>
       <c r="W69" s="3">
@@ -4857,14 +4842,14 @@
       <c r="X69" s="3">
         <v>0.3</v>
       </c>
-      <c r="Y69" s="6" t="s">
+      <c r="Y69" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Z69" s="6"/>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z69" s="3"/>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>165</v>
@@ -4879,22 +4864,22 @@
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="I70" s="3"/>
-      <c r="J70" s="6"/>
-      <c r="K70" s="5"/>
-      <c r="N70" s="6"/>
-      <c r="O70" s="5"/>
-      <c r="Q70" s="6"/>
-      <c r="R70" s="6"/>
-      <c r="S70" s="5"/>
-      <c r="T70" s="6"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="4"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="4"/>
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="4"/>
+      <c r="T70" s="3"/>
       <c r="U70" s="3"/>
       <c r="V70" s="3"/>
       <c r="W70" s="3"/>
       <c r="X70" s="3"/>
-      <c r="Y70" s="6"/>
-      <c r="Z70" s="6"/>
-    </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y70" s="3"/>
+      <c r="Z70" s="3"/>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -4903,24 +4888,24 @@
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
       <c r="I71" s="3"/>
-      <c r="J71" s="6"/>
-      <c r="K71" s="5"/>
-      <c r="N71" s="6"/>
-      <c r="O71" s="5"/>
-      <c r="Q71" s="6"/>
-      <c r="R71" s="6"/>
-      <c r="S71" s="5"/>
-      <c r="T71" s="6"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="4"/>
+      <c r="N71" s="3"/>
+      <c r="O71" s="4"/>
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="4"/>
+      <c r="T71" s="3"/>
       <c r="U71" s="3"/>
       <c r="V71" s="3"/>
       <c r="W71" s="3"/>
       <c r="X71" s="3"/>
-      <c r="Y71" s="6"/>
-      <c r="Z71" s="6"/>
-    </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y71" s="3"/>
+      <c r="Z71" s="3"/>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>18</v>
@@ -4937,30 +4922,30 @@
       <c r="I72" s="3">
         <v>1</v>
       </c>
-      <c r="J72" s="6"/>
-      <c r="K72" s="5"/>
-      <c r="N72" s="6"/>
-      <c r="O72" s="5">
+      <c r="J72" s="3"/>
+      <c r="K72" s="4"/>
+      <c r="N72" s="3"/>
+      <c r="O72" s="4">
         <v>40</v>
       </c>
-      <c r="Q72" s="6" t="s">
+      <c r="Q72" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="R72" s="6" t="s">
+      <c r="R72" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="S72" s="5"/>
-      <c r="T72" s="6"/>
+      <c r="S72" s="4"/>
+      <c r="T72" s="3"/>
       <c r="U72" s="3"/>
       <c r="V72" s="3"/>
       <c r="W72" s="3"/>
       <c r="X72" s="3"/>
-      <c r="Y72" s="6"/>
-      <c r="Z72" s="6"/>
-    </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y72" s="3"/>
+      <c r="Z72" s="3"/>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>166</v>
@@ -4975,26 +4960,26 @@
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="I73" s="3"/>
-      <c r="J73" s="6"/>
-      <c r="K73" s="5"/>
-      <c r="N73" s="6"/>
-      <c r="O73" s="5"/>
-      <c r="Q73" s="6"/>
-      <c r="R73" s="6"/>
-      <c r="S73" s="5"/>
-      <c r="T73" s="6"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="4"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="4"/>
+      <c r="Q73" s="3"/>
+      <c r="R73" s="3"/>
+      <c r="S73" s="4"/>
+      <c r="T73" s="3"/>
       <c r="U73" s="3"/>
       <c r="V73" s="3"/>
       <c r="W73" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="X73" s="3"/>
-      <c r="Y73" s="6"/>
-      <c r="Z73" s="6"/>
-    </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y73" s="3"/>
+      <c r="Z73" s="3"/>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>166</v>
@@ -5009,20 +4994,20 @@
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="I74" s="3"/>
-      <c r="J74" s="6">
+      <c r="J74" s="3">
         <v>0.75</v>
       </c>
-      <c r="K74" s="5" t="s">
+      <c r="K74" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="N74" s="6" t="s">
+      <c r="N74" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="O74" s="5"/>
-      <c r="Q74" s="6"/>
-      <c r="R74" s="6"/>
-      <c r="S74" s="5"/>
-      <c r="T74" s="6"/>
+      <c r="O74" s="4"/>
+      <c r="Q74" s="3"/>
+      <c r="R74" s="3"/>
+      <c r="S74" s="4"/>
+      <c r="T74" s="3"/>
       <c r="U74" s="3"/>
       <c r="V74" s="3"/>
       <c r="W74" s="3">
@@ -5031,12 +5016,12 @@
       <c r="X74" s="3">
         <v>0.25</v>
       </c>
-      <c r="Y74" s="6"/>
-      <c r="Z74" s="6"/>
-    </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y74" s="3"/>
+      <c r="Z74" s="3"/>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>166</v>
@@ -5051,26 +5036,26 @@
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="I75" s="3"/>
-      <c r="J75" s="6"/>
-      <c r="K75" s="5"/>
-      <c r="N75" s="6"/>
-      <c r="O75" s="5"/>
-      <c r="Q75" s="6"/>
-      <c r="R75" s="6"/>
-      <c r="S75" s="5">
+      <c r="J75" s="3"/>
+      <c r="K75" s="4"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="4"/>
+      <c r="Q75" s="3"/>
+      <c r="R75" s="3"/>
+      <c r="S75" s="4">
         <v>26.1</v>
       </c>
-      <c r="T75" s="6"/>
+      <c r="T75" s="3"/>
       <c r="U75" s="3"/>
       <c r="V75" s="3"/>
       <c r="W75" s="3"/>
       <c r="X75" s="3"/>
-      <c r="Y75" s="6" t="s">
+      <c r="Y75" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Z75" s="6"/>
-    </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z75" s="3"/>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -5079,27 +5064,27 @@
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="I76" s="3"/>
-      <c r="J76" s="6"/>
-      <c r="K76" s="5"/>
-      <c r="N76" s="6"/>
-      <c r="O76" s="5"/>
-      <c r="Q76" s="6"/>
-      <c r="R76" s="6"/>
-      <c r="S76" s="5"/>
-      <c r="T76" s="6"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="4"/>
+      <c r="N76" s="3"/>
+      <c r="O76" s="4"/>
+      <c r="Q76" s="3"/>
+      <c r="R76" s="3"/>
+      <c r="S76" s="4"/>
+      <c r="T76" s="3"/>
       <c r="U76" s="3"/>
       <c r="V76" s="3"/>
       <c r="W76" s="3"/>
       <c r="X76" s="3"/>
-      <c r="Y76" s="6"/>
-      <c r="Z76" s="6"/>
-    </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y76" s="3"/>
+      <c r="Z76" s="3"/>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>17</v>
@@ -5111,29 +5096,29 @@
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="I77" s="3"/>
-      <c r="J77" s="6"/>
-      <c r="K77" s="5"/>
-      <c r="N77" s="6"/>
-      <c r="O77" s="5"/>
-      <c r="Q77" s="6"/>
-      <c r="R77" s="6"/>
-      <c r="S77" s="5"/>
-      <c r="T77" s="6"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="4"/>
+      <c r="N77" s="3"/>
+      <c r="O77" s="4"/>
+      <c r="Q77" s="3"/>
+      <c r="R77" s="3"/>
+      <c r="S77" s="4"/>
+      <c r="T77" s="3"/>
       <c r="U77" s="3"/>
       <c r="V77" s="3"/>
       <c r="W77" s="3">
         <v>0.2</v>
       </c>
       <c r="X77" s="3"/>
-      <c r="Y77" s="6"/>
-      <c r="Z77" s="6"/>
-    </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y77" s="3"/>
+      <c r="Z77" s="3"/>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>19</v>
@@ -5145,18 +5130,18 @@
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="I78" s="3"/>
-      <c r="J78" s="6"/>
-      <c r="K78" s="5" t="s">
+      <c r="J78" s="3"/>
+      <c r="K78" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="N78" s="6" t="s">
+      <c r="N78" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="O78" s="5"/>
-      <c r="Q78" s="6"/>
-      <c r="R78" s="6"/>
-      <c r="S78" s="5"/>
-      <c r="T78" s="6"/>
+      <c r="O78" s="4"/>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="4"/>
+      <c r="T78" s="3"/>
       <c r="U78" s="3"/>
       <c r="V78" s="3"/>
       <c r="W78" s="3">
@@ -5165,15 +5150,15 @@
       <c r="X78" s="3">
         <v>0.42</v>
       </c>
-      <c r="Y78" s="6"/>
-      <c r="Z78" s="6"/>
-    </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y78" s="3"/>
+      <c r="Z78" s="3"/>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>131</v>
@@ -5185,30 +5170,30 @@
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="I79" s="3"/>
-      <c r="J79" s="6"/>
-      <c r="K79" s="5"/>
-      <c r="N79" s="6"/>
-      <c r="O79" s="5"/>
-      <c r="Q79" s="6"/>
-      <c r="R79" s="6"/>
-      <c r="S79" s="5"/>
-      <c r="T79" s="6"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="4"/>
+      <c r="N79" s="3"/>
+      <c r="O79" s="4"/>
+      <c r="Q79" s="3"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="4"/>
+      <c r="T79" s="3"/>
       <c r="U79" s="3"/>
       <c r="V79" s="3"/>
       <c r="W79" s="3"/>
       <c r="X79" s="3"/>
-      <c r="Y79" s="6"/>
-      <c r="Z79" s="6"/>
-    </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y79" s="3"/>
+      <c r="Z79" s="3"/>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>121</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>0</v>
@@ -5219,24 +5204,24 @@
       <c r="I80" s="3">
         <v>1</v>
       </c>
-      <c r="J80" s="6">
+      <c r="J80" s="3">
         <v>0.95</v>
       </c>
-      <c r="K80" s="5"/>
-      <c r="N80" s="6"/>
-      <c r="O80" s="5"/>
-      <c r="Q80" s="6"/>
-      <c r="R80" s="6"/>
-      <c r="S80" s="5"/>
-      <c r="T80" s="6"/>
+      <c r="K80" s="4"/>
+      <c r="N80" s="3"/>
+      <c r="O80" s="4"/>
+      <c r="Q80" s="3"/>
+      <c r="R80" s="3"/>
+      <c r="S80" s="4"/>
+      <c r="T80" s="3"/>
       <c r="U80" s="3"/>
       <c r="V80" s="3"/>
       <c r="W80" s="3"/>
       <c r="X80" s="3"/>
-      <c r="Y80" s="6"/>
-      <c r="Z80" s="6"/>
-    </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y80" s="3"/>
+      <c r="Z80" s="3"/>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -5245,22 +5230,22 @@
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="I81" s="3"/>
-      <c r="J81" s="6"/>
-      <c r="K81" s="5"/>
-      <c r="N81" s="6"/>
-      <c r="O81" s="5"/>
-      <c r="Q81" s="6"/>
-      <c r="R81" s="6"/>
-      <c r="S81" s="5"/>
-      <c r="T81" s="6"/>
+      <c r="J81" s="3"/>
+      <c r="K81" s="4"/>
+      <c r="N81" s="3"/>
+      <c r="O81" s="4"/>
+      <c r="Q81" s="3"/>
+      <c r="R81" s="3"/>
+      <c r="S81" s="4"/>
+      <c r="T81" s="3"/>
       <c r="U81" s="3"/>
       <c r="V81" s="3"/>
       <c r="W81" s="3"/>
       <c r="X81" s="3"/>
-      <c r="Y81" s="6"/>
-      <c r="Z81" s="6"/>
-    </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y81" s="3"/>
+      <c r="Z81" s="3"/>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>167</v>
       </c>
@@ -5277,24 +5262,24 @@
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="I82" s="3"/>
-      <c r="J82" s="6"/>
-      <c r="K82" s="5"/>
-      <c r="N82" s="6"/>
-      <c r="O82" s="5"/>
-      <c r="Q82" s="6"/>
-      <c r="R82" s="6"/>
-      <c r="S82" s="5"/>
-      <c r="T82" s="6"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="4"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="4"/>
+      <c r="Q82" s="3"/>
+      <c r="R82" s="3"/>
+      <c r="S82" s="4"/>
+      <c r="T82" s="3"/>
       <c r="U82" s="3"/>
       <c r="V82" s="3"/>
       <c r="W82" s="3">
         <v>0.12</v>
       </c>
       <c r="X82" s="3"/>
-      <c r="Y82" s="6"/>
-      <c r="Z82" s="6"/>
-    </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y82" s="3"/>
+      <c r="Z82" s="3"/>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>167</v>
       </c>
@@ -5311,16 +5296,16 @@
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="I83" s="3"/>
-      <c r="J83" s="6"/>
-      <c r="K83" s="5"/>
-      <c r="N83" s="6" t="s">
+      <c r="J83" s="3"/>
+      <c r="K83" s="4"/>
+      <c r="N83" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="O83" s="5"/>
-      <c r="Q83" s="6"/>
-      <c r="R83" s="6"/>
-      <c r="S83" s="5"/>
-      <c r="T83" s="6"/>
+      <c r="O83" s="4"/>
+      <c r="Q83" s="3"/>
+      <c r="R83" s="3"/>
+      <c r="S83" s="4"/>
+      <c r="T83" s="3"/>
       <c r="U83" s="3"/>
       <c r="V83" s="3"/>
       <c r="W83" s="3">
@@ -5329,10 +5314,10 @@
       <c r="X83" s="3">
         <v>0.45</v>
       </c>
-      <c r="Y83" s="6"/>
-      <c r="Z83" s="6"/>
-    </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y83" s="3"/>
+      <c r="Z83" s="3"/>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>167</v>
       </c>
@@ -5349,22 +5334,22 @@
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="I84" s="3"/>
-      <c r="J84" s="6"/>
-      <c r="K84" s="5"/>
-      <c r="N84" s="6"/>
-      <c r="O84" s="5"/>
-      <c r="Q84" s="6"/>
-      <c r="R84" s="6"/>
-      <c r="S84" s="5"/>
-      <c r="T84" s="6"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="4"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="4"/>
+      <c r="Q84" s="3"/>
+      <c r="R84" s="3"/>
+      <c r="S84" s="4"/>
+      <c r="T84" s="3"/>
       <c r="U84" s="3"/>
       <c r="V84" s="3"/>
       <c r="W84" s="3"/>
       <c r="X84" s="3"/>
-      <c r="Y84" s="6"/>
-      <c r="Z84" s="6"/>
-    </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y84" s="3"/>
+      <c r="Z84" s="3"/>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>167</v>
       </c>
@@ -5383,28 +5368,28 @@
       <c r="I85" s="3">
         <v>1</v>
       </c>
-      <c r="J85" s="6"/>
-      <c r="K85" s="5"/>
-      <c r="N85" s="6"/>
-      <c r="O85" s="5">
+      <c r="J85" s="3"/>
+      <c r="K85" s="4"/>
+      <c r="N85" s="3"/>
+      <c r="O85" s="4">
         <v>30</v>
       </c>
-      <c r="Q85" s="6">
+      <c r="Q85" s="3">
         <v>41</v>
       </c>
-      <c r="R85" s="6">
+      <c r="R85" s="3">
         <v>1020</v>
       </c>
-      <c r="S85" s="5"/>
-      <c r="T85" s="6"/>
+      <c r="S85" s="4"/>
+      <c r="T85" s="3"/>
       <c r="U85" s="3"/>
       <c r="V85" s="3"/>
       <c r="W85" s="3"/>
       <c r="X85" s="3"/>
-      <c r="Y85" s="6"/>
-      <c r="Z85" s="6"/>
-    </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y85" s="3"/>
+      <c r="Z85" s="3"/>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -5413,22 +5398,22 @@
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
       <c r="I86" s="3"/>
-      <c r="J86" s="6"/>
-      <c r="K86" s="5"/>
-      <c r="N86" s="6"/>
-      <c r="O86" s="5"/>
-      <c r="Q86" s="6"/>
-      <c r="R86" s="6"/>
-      <c r="S86" s="5"/>
-      <c r="T86" s="6"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="4"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="4"/>
+      <c r="Q86" s="3"/>
+      <c r="R86" s="3"/>
+      <c r="S86" s="4"/>
+      <c r="T86" s="3"/>
       <c r="U86" s="3"/>
       <c r="V86" s="3"/>
       <c r="W86" s="3"/>
       <c r="X86" s="3"/>
-      <c r="Y86" s="6"/>
-      <c r="Z86" s="6"/>
-    </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Y86" s="3"/>
+      <c r="Z86" s="3"/>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>50</v>
       </c>
@@ -5447,70 +5432,59 @@
       <c r="I87" s="3">
         <v>0.35</v>
       </c>
-      <c r="J87" s="6"/>
-      <c r="K87" s="5" t="s">
+      <c r="J87" s="3"/>
+      <c r="K87" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="N87" s="6"/>
-      <c r="O87" s="5">
+      <c r="N87" s="3"/>
+      <c r="O87" s="4">
         <v>15</v>
       </c>
-      <c r="Q87" s="6"/>
-      <c r="R87" s="6">
+      <c r="Q87" s="3"/>
+      <c r="R87" s="3">
         <v>164</v>
       </c>
-      <c r="S87" s="5"/>
-      <c r="T87" s="6"/>
+      <c r="S87" s="4"/>
+      <c r="T87" s="3"/>
       <c r="U87" s="3"/>
       <c r="V87" s="3"/>
       <c r="W87" s="3"/>
       <c r="X87" s="3"/>
-      <c r="Y87" s="6" t="s">
+      <c r="Y87" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Z87" s="6"/>
-    </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A88" s="4" t="s">
+      <c r="Z87" s="3"/>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>49</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" t="s">
         <v>19</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="C88" t="s">
         <v>133</v>
       </c>
-      <c r="D88" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
-      <c r="I88" s="4">
+      <c r="D88" t="s">
+        <v>0</v>
+      </c>
+      <c r="I88">
         <v>1</v>
       </c>
-      <c r="J88" s="4"/>
-      <c r="K88" s="4"/>
       <c r="N88" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="O88" s="4">
+      <c r="O88">
         <v>15</v>
       </c>
-      <c r="Q88" s="8"/>
-      <c r="R88" s="4" t="s">
+      <c r="Q88" s="3"/>
+      <c r="R88" t="s">
         <v>60</v>
       </c>
-      <c r="S88" s="4"/>
-      <c r="T88" s="4"/>
-      <c r="U88" s="4"/>
-      <c r="V88" s="4"/>
-      <c r="W88" s="4"/>
-      <c r="X88" s="4"/>
-      <c r="Y88" s="4" t="s">
+      <c r="Y88" t="s">
         <v>101</v>
       </c>
-      <c r="Z88" s="6"/>
+      <c r="Z88" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5527,16 +5501,16 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="2" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -5547,7 +5521,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -5558,9 +5532,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>240</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -5569,7 +5543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -5577,7 +5551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>196</v>
       </c>

</xml_diff>

<commit_message>
Added New versions of techmaps compatible with colorconfiguration (older versions will still run)
</commit_message>
<xml_diff>
--- a/Data/Techmap/DEModel.xlsx
+++ b/Data/Techmap/DEModel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janwi\Desktop\5.Semester\Miniforschungsprojekt\Model_Deutschland_Sina\CESM\Data\Techmap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT-OTHER\CESM\Data\Techmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A60DA33-3A9C-48CC-B80B-8056D30B6A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A95DBF7-DB60-447A-BAE2-469B98F4EFFA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{EC78BDD3-7137-425A-8228-7CE92A9A1C25}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="3" xr2:uid="{EC78BDD3-7137-425A-8228-7CE92A9A1C25}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="9" r:id="rId1"/>
@@ -26,19 +26,10 @@
     <definedName name="Energy">Units!$B$3</definedName>
     <definedName name="Power">Units!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -132,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="250">
   <si>
     <t>Base</t>
   </si>
@@ -855,6 +846,33 @@
   </si>
   <si>
     <t>test_tss</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>#00b300</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>#999999</t>
+  </si>
+  <si>
+    <t>#b38033</t>
+  </si>
+  <si>
+    <t>#800000</t>
+  </si>
+  <si>
+    <t>#00ff00</t>
+  </si>
+  <si>
+    <t>#999966</t>
   </si>
 </sst>
 </file>
@@ -958,7 +976,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -978,9 +996,14 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1013,22 +1036,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C14D454B-12DF-41D4-B756-57EA49F00895}" name="Tabelle3" displayName="Tabelle3" ref="A1:B25" totalsRowShown="0">
-  <autoFilter ref="A1:B25" xr:uid="{801D801C-681D-47E7-ACE2-316227FD6501}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C14D454B-12DF-41D4-B756-57EA49F00895}" name="Tabelle3" displayName="Tabelle3" ref="A1:D25" totalsRowShown="0">
+  <autoFilter ref="A1:D25" xr:uid="{801D801C-681D-47E7-ACE2-316227FD6501}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0AF4638F-3EEB-48E0-AC29-8DF8557BEA8D}" name="commodity_name"/>
     <tableColumn id="2" xr3:uid="{C6986DB7-7572-49F8-AEB6-52667D90A759}" name="description"/>
+    <tableColumn id="3" xr3:uid="{EC6EC665-EF07-4D19-809A-3931FAAA9582}" name="color"/>
+    <tableColumn id="4" xr3:uid="{88F5057F-1661-44D9-AA2D-16D91A3A0993}" name="order"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{74A02AEB-67CD-4D1C-8FE9-7365E46D98F4}" name="Tabelle4" displayName="Tabelle4" ref="A1:B61" totalsRowShown="0">
-  <autoFilter ref="A1:B61" xr:uid="{A4F2E66D-1024-44EB-B26C-9EF3C2ACFA7D}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{74A02AEB-67CD-4D1C-8FE9-7365E46D98F4}" name="Tabelle4" displayName="Tabelle4" ref="A1:D61" totalsRowShown="0">
+  <autoFilter ref="A1:D61" xr:uid="{A4F2E66D-1024-44EB-B26C-9EF3C2ACFA7D}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{68045503-4D44-4DCF-9110-03DFC110F65E}" name="conversion_process_name"/>
     <tableColumn id="2" xr3:uid="{B201BB8F-62F7-4A39-95D4-A92A4057D6C7}" name="description"/>
+    <tableColumn id="3" xr3:uid="{67610754-A261-4CC5-966B-0F7D8F54937C}" name="color"/>
+    <tableColumn id="4" xr3:uid="{733EFCD7-4ED0-47BD-A25B-5FA67618576A}" name="order"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1384,12 +1411,12 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>227</v>
       </c>
@@ -1400,7 +1427,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1411,7 +1438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1424,7 +1451,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>203</v>
       </c>
@@ -1436,7 +1463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1448,7 +1475,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1460,7 +1487,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1472,7 +1499,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>204</v>
       </c>
@@ -1502,18 +1529,18 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>223</v>
       </c>
@@ -1539,7 +1566,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1562,7 +1589,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>186</v>
       </c>
@@ -1582,7 +1609,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>197</v>
       </c>
@@ -1605,7 +1632,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1625,7 +1652,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>181</v>
       </c>
@@ -1656,142 +1683,148 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0387EA4-7159-4CF0-ABE0-71D3891C6DB9}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>239</v>
       </c>
       <c r="B1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>121</v>
       </c>
@@ -1807,282 +1840,333 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70369A52-6DA6-442B-A9B0-7FE85C1EDFA1}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>231</v>
       </c>
       <c r="B1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="D4" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D7" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D9" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>144</v>
       </c>
@@ -2107,34 +2191,34 @@
       <selection pane="bottomRight" activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1"/>
-    <col min="11" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="5" width="10.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="9" width="10.88671875" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="11" max="12" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" customWidth="1"/>
+    <col min="14" max="14" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" customWidth="1"/>
     <col min="18" max="18" width="30" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" customWidth="1"/>
-    <col min="20" max="20" width="13.140625" customWidth="1"/>
-    <col min="21" max="21" width="14.140625" customWidth="1"/>
-    <col min="22" max="22" width="14.42578125" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" customWidth="1"/>
-    <col min="24" max="24" width="13.7109375" customWidth="1"/>
-    <col min="25" max="25" width="17.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16.28515625" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" customWidth="1"/>
+    <col min="20" max="20" width="13.109375" customWidth="1"/>
+    <col min="21" max="21" width="14.109375" customWidth="1"/>
+    <col min="22" max="22" width="14.44140625" customWidth="1"/>
+    <col min="23" max="23" width="12.6640625" customWidth="1"/>
+    <col min="24" max="24" width="13.6640625" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" customWidth="1"/>
+    <col min="26" max="26" width="16.33203125" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>231</v>
       </c>
@@ -2214,7 +2298,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="5" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="5" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E2" s="5" t="s">
         <v>201</v>
       </c>
@@ -2273,7 +2357,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H3" s="1" t="s">
         <v>41</v>
       </c>
@@ -2314,7 +2398,7 @@
         <v>TWh/a</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="7"/>
@@ -2339,7 +2423,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>116</v>
       </c>
@@ -2381,7 +2465,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -2421,7 +2505,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>117</v>
       </c>
@@ -2461,7 +2545,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>119</v>
       </c>
@@ -2501,7 +2585,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>120</v>
       </c>
@@ -2541,7 +2625,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>122</v>
       </c>
@@ -2578,7 +2662,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>123</v>
       </c>
@@ -2617,7 +2701,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2641,7 +2725,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>124</v>
       </c>
@@ -2675,7 +2759,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2699,7 +2783,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>126</v>
       </c>
@@ -2736,7 +2820,7 @@
       </c>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
@@ -2773,7 +2857,7 @@
       </c>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>128</v>
       </c>
@@ -2810,7 +2894,7 @@
       </c>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>130</v>
       </c>
@@ -2847,7 +2931,7 @@
       </c>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>132</v>
       </c>
@@ -2884,7 +2968,7 @@
       </c>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>134</v>
       </c>
@@ -2921,7 +3005,7 @@
       </c>
       <c r="Z20" s="3"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>135</v>
       </c>
@@ -2958,7 +3042,7 @@
       </c>
       <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2982,7 +3066,7 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>218</v>
       </c>
@@ -3031,7 +3115,7 @@
       </c>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>219</v>
       </c>
@@ -3080,7 +3164,7 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>220</v>
       </c>
@@ -3129,7 +3213,7 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>221</v>
       </c>
@@ -3178,7 +3262,7 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>222</v>
       </c>
@@ -3227,7 +3311,7 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -3252,7 +3336,7 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>211</v>
       </c>
@@ -3301,7 +3385,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>136</v>
       </c>
@@ -3346,7 +3430,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>212</v>
       </c>
@@ -3395,7 +3479,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>137</v>
       </c>
@@ -3444,7 +3528,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>138</v>
       </c>
@@ -3495,7 +3579,7 @@
       </c>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>217</v>
       </c>
@@ -3544,7 +3628,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>139</v>
       </c>
@@ -3593,7 +3677,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -3617,7 +3701,7 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>140</v>
       </c>
@@ -3661,7 +3745,7 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>141</v>
       </c>
@@ -3701,7 +3785,7 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>142</v>
       </c>
@@ -3745,7 +3829,7 @@
       </c>
       <c r="Z39" s="3"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -3769,7 +3853,7 @@
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>143</v>
       </c>
@@ -3801,7 +3885,7 @@
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -3825,7 +3909,7 @@
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>144</v>
       </c>
@@ -3867,7 +3951,7 @@
       </c>
       <c r="Z43" s="3"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>145</v>
       </c>
@@ -3907,7 +3991,7 @@
       <c r="Y44" s="3"/>
       <c r="Z44" s="3"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>146</v>
       </c>
@@ -3947,7 +4031,7 @@
       <c r="Y45" s="3"/>
       <c r="Z45" s="3"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -3971,7 +4055,7 @@
       <c r="Y46" s="3"/>
       <c r="Z46" s="3"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -3995,7 +4079,7 @@
       <c r="Y47" s="3"/>
       <c r="Z47" s="3"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>147</v>
       </c>
@@ -4042,7 +4126,7 @@
       <c r="Y48" s="3"/>
       <c r="Z48" s="3"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -4067,7 +4151,7 @@
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>149</v>
       </c>
@@ -4114,7 +4198,7 @@
       <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>151</v>
       </c>
@@ -4161,7 +4245,7 @@
       <c r="Y51" s="3"/>
       <c r="Z51" s="3"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>153</v>
       </c>
@@ -4208,7 +4292,7 @@
       <c r="Y52" s="3"/>
       <c r="Z52" s="3"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>155</v>
       </c>
@@ -4255,7 +4339,7 @@
       <c r="Y53" s="3"/>
       <c r="Z53" s="3"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>157</v>
       </c>
@@ -4297,7 +4381,7 @@
       <c r="Y54" s="3"/>
       <c r="Z54" s="3"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>157</v>
       </c>
@@ -4339,7 +4423,7 @@
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>157</v>
       </c>
@@ -4381,7 +4465,7 @@
       <c r="Y56" s="3"/>
       <c r="Z56" s="3"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>157</v>
       </c>
@@ -4423,7 +4507,7 @@
       <c r="Y57" s="3"/>
       <c r="Z57" s="3"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>157</v>
       </c>
@@ -4463,7 +4547,7 @@
       <c r="Y58" s="3"/>
       <c r="Z58" s="3"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -4487,7 +4571,7 @@
       <c r="Y59" s="3"/>
       <c r="Z59" s="3"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>159</v>
       </c>
@@ -4523,7 +4607,7 @@
       </c>
       <c r="Z60" s="3"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>160</v>
       </c>
@@ -4563,7 +4647,7 @@
       </c>
       <c r="Z61" s="3"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>161</v>
       </c>
@@ -4599,7 +4683,7 @@
       </c>
       <c r="Z62" s="3"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>162</v>
       </c>
@@ -4633,7 +4717,7 @@
       </c>
       <c r="Z63" s="3"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>163</v>
       </c>
@@ -4669,7 +4753,7 @@
       </c>
       <c r="Z64" s="3"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>164</v>
       </c>
@@ -4705,7 +4789,7 @@
       </c>
       <c r="Z65" s="3"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -4729,7 +4813,7 @@
       <c r="Y66" s="3"/>
       <c r="Z66" s="3"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>213</v>
       </c>
@@ -4771,7 +4855,7 @@
       <c r="Y67" s="3"/>
       <c r="Z67" s="3"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>213</v>
       </c>
@@ -4805,7 +4889,7 @@
       <c r="Y68" s="3"/>
       <c r="Z68" s="3"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>213</v>
       </c>
@@ -4847,7 +4931,7 @@
       </c>
       <c r="Z69" s="3"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>213</v>
       </c>
@@ -4879,7 +4963,7 @@
       <c r="Y70" s="3"/>
       <c r="Z70" s="3"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -4903,7 +4987,7 @@
       <c r="Y71" s="3"/>
       <c r="Z71" s="3"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>214</v>
       </c>
@@ -4943,7 +5027,7 @@
       <c r="Y72" s="3"/>
       <c r="Z72" s="3"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>214</v>
       </c>
@@ -4977,7 +5061,7 @@
       <c r="Y73" s="3"/>
       <c r="Z73" s="3"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>214</v>
       </c>
@@ -5019,7 +5103,7 @@
       <c r="Y74" s="3"/>
       <c r="Z74" s="3"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>214</v>
       </c>
@@ -5055,7 +5139,7 @@
       </c>
       <c r="Z75" s="3"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -5079,7 +5163,7 @@
       <c r="Y76" s="3"/>
       <c r="Z76" s="3"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>215</v>
       </c>
@@ -5113,7 +5197,7 @@
       <c r="Y77" s="3"/>
       <c r="Z77" s="3"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>215</v>
       </c>
@@ -5153,7 +5237,7 @@
       <c r="Y78" s="3"/>
       <c r="Z78" s="3"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>215</v>
       </c>
@@ -5185,7 +5269,7 @@
       <c r="Y79" s="3"/>
       <c r="Z79" s="3"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>215</v>
       </c>
@@ -5221,7 +5305,7 @@
       <c r="Y80" s="3"/>
       <c r="Z80" s="3"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -5245,7 +5329,7 @@
       <c r="Y81" s="3"/>
       <c r="Z81" s="3"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>167</v>
       </c>
@@ -5279,7 +5363,7 @@
       <c r="Y82" s="3"/>
       <c r="Z82" s="3"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>167</v>
       </c>
@@ -5317,7 +5401,7 @@
       <c r="Y83" s="3"/>
       <c r="Z83" s="3"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>167</v>
       </c>
@@ -5349,7 +5433,7 @@
       <c r="Y84" s="3"/>
       <c r="Z84" s="3"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>167</v>
       </c>
@@ -5389,7 +5473,7 @@
       <c r="Y85" s="3"/>
       <c r="Z85" s="3"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -5413,7 +5497,7 @@
       <c r="Y86" s="3"/>
       <c r="Z86" s="3"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>50</v>
       </c>
@@ -5455,7 +5539,7 @@
       </c>
       <c r="Z87" s="3"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>49</v>
       </c>
@@ -5500,17 +5584,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B2AFB5-A6BC-430C-A010-F2995A75E8FA}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -5521,7 +5605,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -5532,7 +5616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -5543,7 +5627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -5551,7 +5635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>196</v>
       </c>

</xml_diff>

<commit_message>
the column headers changed to input and output
</commit_message>
<xml_diff>
--- a/Data/Techmap/DEModel.xlsx
+++ b/Data/Techmap/DEModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sina Hajikazemi\Documents\mycode\CESM\Data\Techmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02EF5B0-3D7C-42E4-8BAA-9CB331226BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE257E6-BFFC-408A-B957-34D240F6853A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="1440" windowWidth="28800" windowHeight="15370" xr2:uid="{EC78BDD3-7137-425A-8228-7CE92A9A1C25}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{EC78BDD3-7137-425A-8228-7CE92A9A1C25}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="10" r:id="rId1"/>
@@ -412,9 +412,6 @@
     <t>quantity</t>
   </si>
   <si>
-    <t>units</t>
-  </si>
-  <si>
     <t>scale_factor</t>
   </si>
   <si>
@@ -781,7 +778,10 @@
     <t>[2016 14.3;2017 NaN]</t>
   </si>
   <si>
-    <t>unit_calculations</t>
+    <t>input</t>
+  </si>
+  <si>
+    <t>output</t>
   </si>
 </sst>
 </file>
@@ -1335,7 +1335,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1352,10 +1352,10 @@
         <v>119</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>243</v>
@@ -1520,7 +1520,7 @@
         <v>117</v>
       </c>
       <c r="F1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G1" t="s">
         <v>118</v>
@@ -1537,7 +1537,7 @@
         <v>0.05</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E2">
         <v>2015</v>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B3">
         <v>0.05</v>
@@ -1569,7 +1569,7 @@
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -1660,21 +1660,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" t="s">
         <v>141</v>
-      </c>
-      <c r="D1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1698,7 +1698,7 @@
         <v>87</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D7" s="3">
         <v>10</v>
@@ -1714,7 +1714,7 @@
         <v>85</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" s="3">
         <v>10</v>
@@ -1725,7 +1725,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D10" s="3">
         <v>10</v>
@@ -1736,7 +1736,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D11" s="3">
         <v>10</v>
@@ -1747,7 +1747,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D12" s="3">
         <v>10</v>
@@ -1758,7 +1758,7 @@
         <v>46</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D13" s="3">
         <v>10</v>
@@ -1769,7 +1769,7 @@
         <v>47</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D14" s="3">
         <v>10</v>
@@ -1780,7 +1780,7 @@
         <v>79</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D15" s="3">
         <v>10</v>
@@ -1791,7 +1791,7 @@
         <v>72</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D16" s="3">
         <v>10</v>
@@ -1802,7 +1802,7 @@
         <v>48</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D17" s="3">
         <v>10</v>
@@ -1813,7 +1813,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D18" s="3">
         <v>10</v>
@@ -1824,7 +1824,7 @@
         <v>75</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D19" s="3">
         <v>11</v>
@@ -1832,17 +1832,17 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -1870,16 +1870,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" t="s">
         <v>141</v>
-      </c>
-      <c r="D1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1887,7 +1887,7 @@
         <v>70</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -1898,7 +1898,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4" s="3">
         <v>2</v>
@@ -1909,7 +1909,7 @@
         <v>71</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D5" s="3">
         <v>3</v>
@@ -1920,7 +1920,7 @@
         <v>73</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -1931,7 +1931,7 @@
         <v>74</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D7" s="3">
         <v>4</v>
@@ -1942,7 +1942,7 @@
         <v>76</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D8" s="3">
         <v>5</v>
@@ -1953,7 +1953,7 @@
         <v>77</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D9" s="3">
         <v>6</v>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D19" s="8">
         <v>0</v>
@@ -2030,10 +2030,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D22" s="3">
         <v>10</v>
@@ -2041,29 +2041,29 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C25" s="8"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D28">
         <v>10</v>
@@ -2071,10 +2071,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D29" s="3">
         <v>10</v>
@@ -2082,32 +2082,32 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D36" s="3">
         <v>10</v>
@@ -2116,10 +2116,10 @@
     <row r="37" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D38" s="3">
         <v>9</v>
@@ -2127,10 +2127,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D39" s="3">
         <v>11</v>
@@ -2138,10 +2138,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D40" s="3">
         <v>4</v>
@@ -2150,10 +2150,10 @@
     <row r="41" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D42">
         <v>30</v>
@@ -2161,10 +2161,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D43" s="8">
         <v>31</v>
@@ -2172,10 +2172,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D44" s="8">
         <v>32</v>
@@ -2183,10 +2183,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D45">
         <v>33</v>
@@ -2194,10 +2194,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D46" s="3">
         <v>34</v>
@@ -2205,10 +2205,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D47" s="3">
         <v>35</v>
@@ -2216,7 +2216,7 @@
     </row>
     <row r="48" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B48"/>
       <c r="C48"/>
@@ -2225,15 +2225,15 @@
     <row r="49" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D51" s="3">
         <v>10</v>
@@ -2241,15 +2241,15 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D53" s="3">
         <v>9</v>
@@ -2257,10 +2257,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D54" s="3">
         <v>3</v>
@@ -2271,7 +2271,7 @@
         <v>50</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D56" s="3">
         <v>10</v>
@@ -2282,7 +2282,7 @@
         <v>49</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D57" s="3">
         <v>10</v>
@@ -2294,27 +2294,27 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2367,16 +2367,16 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
         <v>123</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>124</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>125</v>
-      </c>
-      <c r="D1" t="s">
-        <v>126</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>103</v>
@@ -2462,13 +2462,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>98</v>
@@ -2492,7 +2492,7 @@
         <v>67</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="X2" s="6" t="s">
         <v>69</v>
@@ -2617,7 +2617,7 @@
       <c r="N5" s="5"/>
       <c r="O5" s="4"/>
       <c r="P5" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -2657,7 +2657,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="4"/>
       <c r="P6" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
@@ -2737,7 +2737,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="4"/>
       <c r="P8" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
@@ -2828,13 +2828,13 @@
     </row>
     <row r="11" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>0</v>
@@ -2853,7 +2853,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="4"/>
       <c r="P11" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
@@ -2928,13 +2928,13 @@
     </row>
     <row r="14" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>0</v>
@@ -2962,13 +2962,13 @@
     </row>
     <row r="15" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>0</v>
@@ -3044,7 +3044,7 @@
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
       <c r="T17" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
@@ -3242,7 +3242,7 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>79</v>
@@ -3303,7 +3303,7 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>45</v>
@@ -3324,11 +3324,11 @@
         <v>0.86</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L25" s="5"/>
       <c r="N25" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O25" s="4">
         <v>30</v>
@@ -3337,7 +3337,7 @@
         <v>165</v>
       </c>
       <c r="R25" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="S25" s="4"/>
       <c r="T25" s="5"/>
@@ -3350,7 +3350,7 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>18</v>
@@ -3371,11 +3371,11 @@
         <v>0.86</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L26" s="4"/>
       <c r="N26" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O26" s="4">
         <v>40</v>
@@ -3397,10 +3397,10 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>19</v>
@@ -3418,11 +3418,11 @@
         <v>0.95</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L27" s="4"/>
       <c r="N27" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O27" s="4">
         <v>25</v>
@@ -3444,7 +3444,7 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>48</v>
@@ -3465,11 +3465,11 @@
         <v>0.76</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L28" s="4"/>
       <c r="N28" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O28" s="4">
         <v>40</v>
@@ -3491,7 +3491,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>47</v>
@@ -3512,11 +3512,11 @@
         <v>0.95</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L29" s="4"/>
       <c r="N29" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O29" s="4">
         <v>60</v>
@@ -3565,7 +3565,7 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>17</v>
@@ -3584,11 +3584,11 @@
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L31" s="5"/>
       <c r="N31" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O31" s="4"/>
       <c r="Q31" s="5">
@@ -3608,7 +3608,7 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>17</v>
@@ -3631,7 +3631,7 @@
       </c>
       <c r="L32" s="5"/>
       <c r="N32" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O32" s="4">
         <v>25</v>
@@ -3640,7 +3640,7 @@
         <v>15</v>
       </c>
       <c r="R32" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="S32" s="4"/>
       <c r="T32" s="5"/>
@@ -3655,7 +3655,7 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>17</v>
@@ -3700,7 +3700,7 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>17</v>
@@ -3719,13 +3719,13 @@
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O34" s="4"/>
       <c r="Q34" s="5">
@@ -3745,7 +3745,7 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>17</v>
@@ -3768,7 +3768,7 @@
       </c>
       <c r="L35" s="5"/>
       <c r="N35" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O35" s="4">
         <v>25</v>
@@ -3777,7 +3777,7 @@
         <v>93</v>
       </c>
       <c r="R35" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="S35" s="4"/>
       <c r="T35" s="5"/>
@@ -3792,7 +3792,7 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>17</v>
@@ -3811,13 +3811,13 @@
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O36" s="4"/>
       <c r="Q36" s="5">
@@ -3837,7 +3837,7 @@
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>17</v>
@@ -3860,7 +3860,7 @@
       </c>
       <c r="L37" s="5"/>
       <c r="N37" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O37" s="4">
         <v>25</v>
@@ -3869,7 +3869,7 @@
         <v>13</v>
       </c>
       <c r="R37" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="S37" s="4"/>
       <c r="T37" s="5"/>
@@ -3884,7 +3884,7 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>18</v>
@@ -3928,7 +3928,7 @@
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>19</v>
@@ -3972,10 +3972,10 @@
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>83</v>
@@ -4012,7 +4012,7 @@
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>83</v>
@@ -4044,7 +4044,7 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>45</v>
@@ -4084,7 +4084,7 @@
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>19</v>
@@ -4111,7 +4111,7 @@
         <v>1.5</v>
       </c>
       <c r="R47" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="S47" s="4"/>
       <c r="T47" s="5"/>
@@ -4124,7 +4124,7 @@
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>46</v>
@@ -4209,13 +4209,13 @@
       </c>
       <c r="J50" s="5"/>
       <c r="K50" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="N50" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="L50" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="N50" s="4" t="s">
-        <v>216</v>
       </c>
       <c r="O50" s="4">
         <v>25</v>
@@ -4224,15 +4224,15 @@
         <v>1.93</v>
       </c>
       <c r="R50" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="S50" s="4"/>
       <c r="T50" s="5"/>
       <c r="U50" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="V50" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="W50" s="2"/>
       <c r="X50" s="2"/>
@@ -4266,7 +4266,7 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>45</v>
@@ -4285,10 +4285,10 @@
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>92</v>
@@ -4300,12 +4300,12 @@
         <v>20</v>
       </c>
       <c r="R52" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S52" s="4"/>
       <c r="T52" s="5"/>
       <c r="U52" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V52" s="2"/>
       <c r="W52" s="2"/>
@@ -4317,10 +4317,10 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>81</v>
@@ -4336,10 +4336,10 @@
       </c>
       <c r="J53" s="5"/>
       <c r="K53" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>93</v>
@@ -4351,12 +4351,12 @@
         <v>10</v>
       </c>
       <c r="R53" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S53" s="4"/>
       <c r="T53" s="5"/>
       <c r="U53" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V53" s="2">
         <v>0.55000000000000004</v>
@@ -4370,7 +4370,7 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>19</v>
@@ -4400,12 +4400,12 @@
         <v>18</v>
       </c>
       <c r="R54" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="S54" s="4"/>
       <c r="T54" s="5"/>
       <c r="U54" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="V54" s="2"/>
       <c r="W54" s="2"/>
@@ -4417,7 +4417,7 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A55" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>79</v>
@@ -4436,10 +4436,10 @@
       </c>
       <c r="J55" s="5"/>
       <c r="K55" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N55" s="4" t="s">
         <v>94</v>
@@ -4451,12 +4451,12 @@
         <v>15</v>
       </c>
       <c r="R55" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="S55" s="4"/>
       <c r="T55" s="5"/>
       <c r="U55" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V55" s="2"/>
       <c r="W55" s="2"/>
@@ -4468,7 +4468,7 @@
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A56" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>19</v>
@@ -4498,12 +4498,12 @@
         <v>15</v>
       </c>
       <c r="R56" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="S56" s="4"/>
       <c r="T56" s="5"/>
       <c r="U56" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V56" s="2"/>
       <c r="W56" s="2"/>
@@ -4563,7 +4563,7 @@
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>45</v>
@@ -4597,7 +4597,7 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>90</v>
@@ -4633,7 +4633,7 @@
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>90</v>
@@ -4683,7 +4683,7 @@
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>90</v>
@@ -4741,7 +4741,7 @@
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>18</v>
@@ -4775,7 +4775,7 @@
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>91</v>
@@ -4809,7 +4809,7 @@
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>91</v>
@@ -4828,10 +4828,10 @@
         <v>0.75</v>
       </c>
       <c r="K66" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="L66" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="L66" s="4" t="s">
-        <v>178</v>
       </c>
       <c r="N66" s="5"/>
       <c r="O66" s="4">
@@ -4859,7 +4859,7 @@
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>91</v>
@@ -4917,13 +4917,13 @@
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>0</v>
@@ -4953,10 +4953,10 @@
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>17</v>
@@ -4987,10 +4987,10 @@
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>19</v>
@@ -5004,11 +5004,11 @@
       <c r="I71" s="2"/>
       <c r="J71" s="5"/>
       <c r="K71" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L71" s="4"/>
       <c r="N71" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O71" s="4">
         <v>30</v>
@@ -5034,10 +5034,10 @@
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>85</v>
@@ -5085,10 +5085,10 @@
       </c>
       <c r="J74" s="5"/>
       <c r="K74" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N74" s="5"/>
       <c r="O74" s="4">
@@ -5142,7 +5142,7 @@
         <v>450</v>
       </c>
       <c r="R75" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S75" s="3"/>
       <c r="T75" s="3"/>
@@ -5157,13 +5157,13 @@
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A76" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B76" t="s">
         <v>19</v>
       </c>
       <c r="C76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D76" t="s">
         <v>0</v>
@@ -5172,10 +5172,10 @@
         <v>0.7</v>
       </c>
       <c r="Q76" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="R76" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S76">
         <v>0</v>
@@ -5188,13 +5188,13 @@
     </row>
     <row r="78" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>0</v>
@@ -5208,10 +5208,10 @@
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>87</v>
@@ -5222,10 +5222,10 @@
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A80" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>81</v>
@@ -5236,10 +5236,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>85</v>
@@ -5250,10 +5250,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>83</v>
@@ -5264,10 +5264,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>19</v>
@@ -5278,10 +5278,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>45</v>
@@ -5292,10 +5292,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>46</v>
@@ -5306,10 +5306,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>47</v>
@@ -5320,10 +5320,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>79</v>
@@ -5334,10 +5334,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>72</v>
@@ -5348,10 +5348,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>48</v>
@@ -5362,10 +5362,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>18</v>
@@ -5376,10 +5376,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>75</v>
@@ -5390,13 +5390,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>0</v>
@@ -5404,13 +5404,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>0</v>
@@ -5463,7 +5463,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>

</xml_diff>